<commit_message>
FEAT: Hibernate configuration for EventBuddy is added
</commit_message>
<xml_diff>
--- a/ProfileManager/Tasks_Tracking.xlsx
+++ b/ProfileManager/Tasks_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JAVA\GitHubWorkspace\Projects\ProfileManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C4E3E5-1392-44CB-A26E-1AE6CC82203A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D760E4-BF37-4D76-8A73-7535597BB107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>STATUS</t>
   </si>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,22 +484,24 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="3">
         <v>45655</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="7">
         <v>45657</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">

</xml_diff>